<commit_message>
- Added extra FHIR sessions by PA and Decor guys
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@558 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Baltimore WGM/FHIR track planning sheet.xlsx
+++ b/documents/Baltimore WGM/FHIR track planning sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15315" windowHeight="8070"/>
+    <workbookView xWindow="360" yWindow="312" windowWidth="15312" windowHeight="8076"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Pharmacy: Pharmacy resources &amp; extensions</t>
   </si>
   <si>
-    <t>MnM: data types, narrative</t>
-  </si>
-  <si>
     <t>PA: Patient Administration resources</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>ITS + SOA: REST and related issues</t>
   </si>
   <si>
-    <t>ITS: XML/JSON/ATOM</t>
-  </si>
-  <si>
     <t>CGIT &amp; Templates</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>?FHIR governance/management groups</t>
   </si>
   <si>
-    <t>OO: Diagnostic data/reports</t>
-  </si>
-  <si>
     <t>Tooling &amp; Pubs v3: FHIR tooling &amp; publication issues</t>
   </si>
   <si>
@@ -118,6 +109,15 @@
   </si>
   <si>
     <t>Devices: Device &amp; data registries (use Devices room if big enough for 25+)</t>
+  </si>
+  <si>
+    <t>ITS: XML/JSON/ATOM; PA: Patient vs. Person</t>
+  </si>
+  <si>
+    <t>OO: Diagnostic data/reports; PA: Scheduling</t>
+  </si>
+  <si>
+    <t>MnM: data types, narrative; Decor discussion</t>
   </si>
 </sst>
 </file>
@@ -465,19 +465,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="36.5703125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="36.5546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,34 +485,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -520,42 +520,42 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -563,34 +563,34 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -598,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -606,34 +606,34 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -641,34 +641,34 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -679,28 +679,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +716,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -729,7 +729,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>